<commit_message>
offer letter, get i2c io expander working, finland figures, exam 4 review done
</commit_message>
<xml_diff>
--- a/HON 394/States Gun Regulations.xlsx
+++ b/HON 394/States Gun Regulations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\Junior\HON 394\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18DE879-278B-4CC9-B037-9F184585E091}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D7C8D1-AD62-4EE6-B86C-5A26B21C3AE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7365" xr2:uid="{6FB77C70-E30F-4A1F-9DB5-2F2CD4661C80}"/>
   </bookViews>
@@ -161,6 +161,64 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0743494242460454E-16"/>
+                  <c:y val="1.6146788290972124E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="3.5527192505645594E-2"/>
+                      <c:h val="8.2701910740363621E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-1752-45D3-A4F2-5DB73FDA5FA0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -175,7 +233,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -335,9 +393,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2400"/>
                   <a:t>Legislation</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US" sz="2000"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -392,7 +451,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -456,7 +515,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2400"/>
                   <a:t># of States</a:t>
                 </a:r>
               </a:p>
@@ -507,7 +566,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1105,7 +1164,7 @@
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -1114,7 +1173,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8665882" cy="6293971"/>
+    <xdr:ext cx="8668712" cy="6292273"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">

</xml_diff>

<commit_message>
software demo, finish latex figs, inertia comparison same
</commit_message>
<xml_diff>
--- a/HON 394/States Gun Regulations.xlsx
+++ b/HON 394/States Gun Regulations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\Junior\HON 394\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D7C8D1-AD62-4EE6-B86C-5A26B21C3AE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04B8C0F-614C-49D8-A2E1-DD30666AFFB3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7365" xr2:uid="{6FB77C70-E30F-4A1F-9DB5-2F2CD4661C80}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7365" activeTab="1" xr2:uid="{6FB77C70-E30F-4A1F-9DB5-2F2CD4661C80}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
@@ -52,13 +52,13 @@
     <t>Restrictions on Long Gun Ownership</t>
   </si>
   <si>
-    <t>Restrictions on Handgin Ownership</t>
-  </si>
-  <si>
     <t>Restrictions on Carrying Long Guns</t>
   </si>
   <si>
     <t>Restrictions on Carrying Handguns</t>
+  </si>
+  <si>
+    <t>Restrictions on Handgun Ownership</t>
   </si>
 </sst>
 </file>
@@ -129,7 +129,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.58896348260070586"/>
+          <c:y val="2.22404384025029E-2"/>
+          <c:w val="0.38449485124754701"/>
+          <c:h val="0.83466932511811553"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -165,8 +175,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.0743494242460454E-16"/>
-                  <c:y val="1.6146788290972124E-2"/>
+                  <c:x val="-3.5936597892519143E-2"/>
+                  <c:y val="-6.877125078115312E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -209,8 +219,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="3.5527192505645594E-2"/>
-                      <c:h val="8.2701910740363621E-2"/>
+                      <c:w val="4.8728325882496024E-2"/>
+                      <c:h val="8.2701953767589167E-2"/>
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
@@ -300,7 +310,7 @@
                   <c:v>Restrictions on Long Gun Ownership</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Restrictions on Handgin Ownership</c:v>
+                  <c:v>Restrictions on Handgun Ownership</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Restrictions on Carrying Long Guns</c:v>
@@ -429,7 +439,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -451,7 +461,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -478,6 +488,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1161,7 +1172,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CEEE92F3-8CBB-46A5-8327-AB854B22E8A9}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="102" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="300" r:id="rId1"/>
@@ -1173,7 +1184,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668712" cy="6292273"/>
+    <xdr:ext cx="8658311" cy="6281351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1501,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC00BA6D-1457-49B0-9755-CD31D888BB16}">
   <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,7 +1580,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>16</v>
@@ -1577,7 +1588,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>9</v>
@@ -1585,7 +1596,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>28</v>

</xml_diff>